<commit_message>
Added pytests to rows and cols
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rows and cols" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="math" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="data convert" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -154,30 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">John Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maths title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Works on the xlsxopera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YYY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZZZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$</t>
   </si>
 </sst>
 </file>
@@ -188,7 +164,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -256,38 +232,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Roboto"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,23 +273,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF972F"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE06666"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -365,13 +299,6 @@
       <bottom style="thick"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -398,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -465,50 +392,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -543,7 +426,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFE06666"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -590,11 +473,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
@@ -640,11 +523,11 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.94"/>
@@ -808,287 +691,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.73"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="19"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="n">
-        <v>44456</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="n">
-        <v>44572</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="n">
-        <v>44625</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="n">
-        <v>44630</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="n">
-        <v>44714</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added value rows and cols
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -477,7 +477,7 @@
       <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
@@ -524,10 +524,10 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.94"/>
@@ -697,7 +697,7 @@
       <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.73"/>

</xml_diff>